<commit_message>
Arranged initially by batting order
</commit_message>
<xml_diff>
--- a/mls_f15.xlsx
+++ b/mls_f15.xlsx
@@ -58,46 +58,46 @@
     <t>OPS</t>
   </si>
   <si>
+    <t>Andrew Burch</t>
+  </si>
+  <si>
     <t>Oliver Patton</t>
   </si>
   <si>
     <t>Rich Squitieri</t>
   </si>
   <si>
-    <t>Andrew Burch</t>
-  </si>
-  <si>
     <t>Luke Heuer</t>
   </si>
   <si>
+    <t>Derek Bayes</t>
+  </si>
+  <si>
+    <t>Joe Edwards</t>
+  </si>
+  <si>
+    <t>Nick Mirman</t>
+  </si>
+  <si>
     <t>Nick Hanten</t>
   </si>
   <si>
     <t>Scott Richardson</t>
   </si>
   <si>
+    <t>Charlie Henschen</t>
+  </si>
+  <si>
+    <t>Gordon Walker</t>
+  </si>
+  <si>
     <t>Amory Meltzer</t>
   </si>
   <si>
-    <t>Gordon Walker</t>
-  </si>
-  <si>
-    <t>Charlie Henschen</t>
-  </si>
-  <si>
-    <t>Joe Edwards</t>
-  </si>
-  <si>
-    <t>Nick Mirman</t>
+    <t>Andrew Scott</t>
   </si>
   <si>
     <t>Qaiser Patel</t>
-  </si>
-  <si>
-    <t>Derek Bayes</t>
-  </si>
-  <si>
-    <t>Andrew Scott</t>
   </si>
   <si>
     <t>Brett Smith</t>
@@ -275,59 +275,55 @@
         <v>15</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f t="shared" ref="B2:C2" si="1">4+4+3</f>
+        <f t="shared" ref="B2:B3" si="1">4+4+3</f>
         <v>11</v>
       </c>
       <c r="C2" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <f>4+2+3</f>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="str">
-        <f t="shared" ref="D2:E2" si="2">3+3+1</f>
-        <v>7</v>
+        <f>4+2+2</f>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="F2" s="3" t="str">
-        <f>2+4</f>
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="str">
-        <f>2+1
-</f>
-        <v>3</v>
+        <f>3+3+2</f>
+        <v>8</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.0</v>
       </c>
       <c r="H2" s="3">
         <v>0.0</v>
       </c>
-      <c r="I2" s="3" t="str">
-        <f>0+2</f>
-        <v>2</v>
+      <c r="I2" s="3">
+        <v>1.0</v>
       </c>
       <c r="J2" s="3">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="K2" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="5" t="str">
-        <f t="shared" ref="M2:M17" si="4">IF(C2,D2/C2,)</f>
-        <v>0.636</v>
+        <f t="shared" ref="M2:M17" si="3">IF(C2,D2/C2,)</f>
+        <v>0.889</v>
       </c>
       <c r="N2" s="5" t="str">
-        <f t="shared" ref="N2:N17" si="5">IF(C2,((D2-G2-H2-I2)+(2*G2)+(3*H2)+(4*I2))/C2,)</f>
-        <v>1.455</v>
+        <f t="shared" ref="N2:N17" si="4">IF(C2,((D2-G2-H2-I2)+(2*G2)+(3*H2)+(4*I2))/C2,)</f>
+        <v>1.444</v>
       </c>
       <c r="O2" s="5" t="str">
-        <f t="shared" ref="O2:O18" si="6">IF(B2,(D2+J2)/(C2+J2),)</f>
-        <v>0.636</v>
+        <f t="shared" ref="O2:O18" si="5">IF(B2,(D2+J2)/(C2+J2),)</f>
+        <v>0.909</v>
       </c>
       <c r="P2" s="5" t="str">
-        <f t="shared" ref="P2:P18" si="7">IF(N2,N2+O2,)</f>
-        <v>2.091</v>
+        <f t="shared" ref="P2:P18" si="6">IF(N2,N2+O2,)</f>
+        <v>2.354</v>
       </c>
     </row>
     <row r="3">
@@ -335,57 +331,59 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="str">
-        <f t="shared" ref="B3:C3" si="3">4+3+3</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>10</v>
+        <f>4+4+3</f>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f>3+3+2</f>
-        <v>8</v>
+        <f t="shared" ref="D3:E3" si="2">3+3+1</f>
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <f>2+4</f>
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="str">
         <f>2+1
 </f>
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="str">
-        <f>3+1+3</f>
-        <v>7</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1.0</v>
-      </c>
       <c r="H3" s="3">
         <v>0.0</v>
       </c>
-      <c r="I3" s="3">
-        <v>0.0</v>
+      <c r="I3" s="3" t="str">
+        <f>0+2</f>
+        <v>2</v>
       </c>
       <c r="J3" s="3">
         <v>0.0</v>
       </c>
       <c r="K3" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.800</v>
+        <f t="shared" si="3"/>
+        <v>0.636</v>
       </c>
       <c r="N3" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.900</v>
+        <f t="shared" si="4"/>
+        <v>1.455</v>
       </c>
       <c r="O3" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.800</v>
+        <f t="shared" si="5"/>
+        <v>0.636</v>
       </c>
       <c r="P3" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>1.700</v>
+        <f t="shared" si="6"/>
+        <v>2.091</v>
       </c>
     </row>
     <row r="4">
@@ -393,55 +391,57 @@
         <v>17</v>
       </c>
       <c r="B4" s="3" t="str">
-        <f>4+4+3</f>
-        <v>11</v>
+        <f t="shared" ref="B4:C4" si="7">4+3+3</f>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f>4+2+3</f>
-        <v>9</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>4+2+2</f>
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="str">
         <f>3+3+2</f>
         <v>8</v>
       </c>
-      <c r="F4" s="3">
-        <v>3.0</v>
+      <c r="E4" s="3" t="str">
+        <f>2+1
+</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f>3+1+3</f>
+        <v>7</v>
       </c>
       <c r="G4" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" s="3">
         <v>0.0</v>
       </c>
       <c r="I4" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J4" s="3">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K4" s="3">
         <v>0.0</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.889</v>
+        <f t="shared" si="3"/>
+        <v>0.800</v>
       </c>
       <c r="N4" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>1.444</v>
+        <f t="shared" si="4"/>
+        <v>0.900</v>
       </c>
       <c r="O4" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.909</v>
+        <f t="shared" si="5"/>
+        <v>0.800</v>
       </c>
       <c r="P4" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>2.354</v>
+        <f t="shared" si="6"/>
+        <v>1.700</v>
       </c>
     </row>
     <row r="5">
@@ -487,19 +487,19 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.714</v>
       </c>
       <c r="N5" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.571</v>
       </c>
       <c r="O5" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.714</v>
       </c>
       <c r="P5" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2.286</v>
       </c>
     </row>
@@ -508,24 +508,26 @@
         <v>19</v>
       </c>
       <c r="B6" s="3" t="str">
-        <f t="shared" ref="B6:C6" si="9">4+4+3</f>
-        <v>11</v>
+        <f t="shared" ref="B6:B7" si="10">4+3
+</f>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="str">
+        <f>4+2
+</f>
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" ref="D6:E6" si="9">2+2
+</f>
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>2+2+2</f>
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="str">
-        <f>1+2+1</f>
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="str">
-        <f>1+1+1</f>
-        <v>3</v>
+      <c r="F6" s="3">
+        <v>1.0</v>
       </c>
       <c r="G6" s="3">
         <v>0.0</v>
@@ -537,27 +539,27 @@
         <v>0.0</v>
       </c>
       <c r="J6" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K6" s="3">
         <v>0.0</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.545</v>
+        <f t="shared" si="3"/>
+        <v>0.667</v>
       </c>
       <c r="N6" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.545</v>
+        <f t="shared" si="4"/>
+        <v>0.667</v>
       </c>
       <c r="O6" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.545</v>
+        <f t="shared" si="5"/>
+        <v>0.714</v>
       </c>
       <c r="P6" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>1.091</v>
+        <f t="shared" si="6"/>
+        <v>1.381</v>
       </c>
     </row>
     <row r="7">
@@ -565,16 +567,18 @@
         <v>20</v>
       </c>
       <c r="B7" s="3" t="str">
-        <f t="shared" ref="B7:C7" si="10">3+3+3</f>
-        <v>9</v>
+        <f t="shared" si="10"/>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>9</v>
+        <f>4+3
+</f>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>1+1+1</f>
-        <v>3</v>
+        <f>3+2
+</f>
+        <v>5</v>
       </c>
       <c r="E7" s="3">
         <v>1.0</v>
@@ -588,7 +592,7 @@
         <v>1.0</v>
       </c>
       <c r="H7" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I7" s="3">
         <v>0.0</v>
@@ -601,46 +605,40 @@
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.333</v>
+        <f t="shared" si="3"/>
+        <v>0.714</v>
       </c>
       <c r="N7" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.444</v>
+        <f t="shared" si="4"/>
+        <v>1.143</v>
       </c>
       <c r="O7" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.333</v>
+        <f t="shared" si="5"/>
+        <v>0.714</v>
       </c>
       <c r="P7" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>0.778</v>
+        <f t="shared" si="6"/>
+        <v>1.857</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="3" t="str">
-        <f t="shared" ref="B8:C8" si="11">3+3+3</f>
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="str">
-        <f t="shared" si="11"/>
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f>2+2+1</f>
-        <v>5</v>
-      </c>
-      <c r="E8" s="3" t="str">
-        <f>2+1
-</f>
-        <v>3</v>
-      </c>
-      <c r="F8" s="3" t="str">
-        <f>0+2</f>
-        <v>2</v>
+      <c r="B8" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2.0</v>
       </c>
       <c r="G8" s="3">
         <v>0.0</v>
@@ -659,20 +657,20 @@
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.556</v>
+        <f t="shared" si="3"/>
+        <v>0.667</v>
       </c>
       <c r="N8" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.556</v>
+        <f t="shared" si="4"/>
+        <v>0.667</v>
       </c>
       <c r="O8" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.556</v>
+        <f t="shared" si="5"/>
+        <v>0.667</v>
       </c>
       <c r="P8" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>1.111</v>
+        <f t="shared" si="6"/>
+        <v>1.333</v>
       </c>
     </row>
     <row r="9">
@@ -680,24 +678,24 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="str">
-        <f t="shared" ref="B9:C9" si="12">3+3+3</f>
-        <v>9</v>
+        <f t="shared" ref="B9:C9" si="11">4+4+3</f>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>9</v>
+        <f t="shared" si="11"/>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="str">
+        <f>2+2+2</f>
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="str">
         <f>1+2+1</f>
         <v>4</v>
       </c>
-      <c r="E9" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1.0</v>
+      <c r="F9" s="3" t="str">
+        <f>1+1+1</f>
+        <v>3</v>
       </c>
       <c r="G9" s="3">
         <v>0.0</v>
@@ -716,20 +714,20 @@
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.444</v>
+        <f t="shared" si="3"/>
+        <v>0.545</v>
       </c>
       <c r="N9" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.444</v>
+        <f t="shared" si="4"/>
+        <v>0.545</v>
       </c>
       <c r="O9" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.444</v>
+        <f t="shared" si="5"/>
+        <v>0.545</v>
       </c>
       <c r="P9" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>0.889</v>
+        <f t="shared" si="6"/>
+        <v>1.091</v>
       </c>
     </row>
     <row r="10">
@@ -737,31 +735,30 @@
         <v>23</v>
       </c>
       <c r="B10" s="3" t="str">
-        <f t="shared" ref="B10:C10" si="13">3+3+3</f>
+        <f t="shared" ref="B10:C10" si="12">3+3+3</f>
         <v>9</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="D10" s="3" t="str">
-        <f>2+2
-</f>
-        <v>4</v>
-      </c>
-      <c r="E10" s="3" t="str">
-        <f t="shared" ref="E10:F10" si="14">2+1+1</f>
-        <v>4</v>
+        <f>1+1+1</f>
+        <v>3</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.0</v>
       </c>
       <c r="F10" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v>4</v>
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="G10" s="3">
         <v>1.0</v>
       </c>
       <c r="H10" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I10" s="3">
         <v>0.0</v>
@@ -774,20 +771,20 @@
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.333</v>
+      </c>
+      <c r="N10" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.444</v>
       </c>
-      <c r="N10" s="5" t="str">
-        <f t="shared" si="5"/>
+      <c r="O10" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>0.333</v>
+      </c>
+      <c r="P10" s="5" t="str">
+        <f t="shared" si="6"/>
         <v>0.778</v>
-      </c>
-      <c r="O10" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.444</v>
-      </c>
-      <c r="P10" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>1.222</v>
       </c>
     </row>
     <row r="11">
@@ -795,26 +792,25 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="str">
-        <f t="shared" ref="B11:C11" si="15">4+3
-</f>
-        <v>7</v>
+        <f t="shared" ref="B11:C11" si="13">3+3+3</f>
+        <v>9</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v>7</v>
+        <f t="shared" si="13"/>
+        <v>9</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f>3+2
-</f>
-        <v>5</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1.0</v>
+        <f>2+2
+</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="3" t="str">
+        <f t="shared" ref="E11:F11" si="14">2+1+1</f>
+        <v>4</v>
       </c>
       <c r="F11" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
+        <f t="shared" si="14"/>
+        <v>4</v>
       </c>
       <c r="G11" s="3">
         <v>1.0</v>
@@ -833,40 +829,45 @@
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.714</v>
+        <f t="shared" si="3"/>
+        <v>0.444</v>
       </c>
       <c r="N11" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>1.143</v>
+        <f t="shared" si="4"/>
+        <v>0.778</v>
       </c>
       <c r="O11" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.714</v>
+        <f t="shared" si="5"/>
+        <v>0.444</v>
       </c>
       <c r="P11" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>1.857</v>
+        <f t="shared" si="6"/>
+        <v>1.222</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="C12" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D12" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0.0</v>
+      <c r="B12" s="3" t="str">
+        <f t="shared" ref="B12:C12" si="15">3+3+3</f>
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>1+2+1</f>
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="str">
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="F12" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G12" s="3">
         <v>0.0</v>
@@ -885,40 +886,46 @@
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.667</v>
+        <f t="shared" si="3"/>
+        <v>0.444</v>
       </c>
       <c r="N12" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.667</v>
+        <f t="shared" si="4"/>
+        <v>0.444</v>
       </c>
       <c r="O12" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.667</v>
+        <f t="shared" si="5"/>
+        <v>0.444</v>
       </c>
       <c r="P12" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>1.333</v>
+        <f t="shared" si="6"/>
+        <v>0.889</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.0</v>
+      <c r="B13" s="3" t="str">
+        <f t="shared" ref="B13:C13" si="16">3+3+3</f>
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>2+2+1</f>
+        <v>5</v>
+      </c>
+      <c r="E13" s="3" t="str">
+        <f>2+1
+</f>
+        <v>3</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f>0+2</f>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
         <v>0.0</v>
@@ -937,47 +944,40 @@
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>0.556</v>
       </c>
       <c r="N13" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>0.556</v>
       </c>
       <c r="O13" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>0.556</v>
       </c>
       <c r="P13" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v/>
+        <f t="shared" si="6"/>
+        <v>1.111</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="3" t="str">
-        <f>4+3
-</f>
-        <v>7</v>
-      </c>
-      <c r="C14" s="3" t="str">
-        <f>4+2
-</f>
-        <v>6</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" ref="D14:E14" si="16">2+2
-</f>
-        <v>4</v>
-      </c>
-      <c r="E14" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v>4</v>
+      <c r="B14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.0</v>
       </c>
       <c r="F14" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G14" s="3">
         <v>0.0</v>
@@ -989,27 +989,27 @@
         <v>0.0</v>
       </c>
       <c r="J14" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K14" s="3">
         <v>0.0</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
+        <v>0.333</v>
+      </c>
+      <c r="N14" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>0.333</v>
+      </c>
+      <c r="O14" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>0.333</v>
+      </c>
+      <c r="P14" s="5" t="str">
+        <f t="shared" si="6"/>
         <v>0.667</v>
-      </c>
-      <c r="N14" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.667</v>
-      </c>
-      <c r="O14" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.714</v>
-      </c>
-      <c r="P14" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>1.381</v>
       </c>
     </row>
     <row r="15">
@@ -1017,13 +1017,13 @@
         <v>28</v>
       </c>
       <c r="B15" s="3">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="C15" s="3">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="D15" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E15" s="3">
         <v>0.0</v>
@@ -1048,20 +1048,20 @@
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.333</v>
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="N15" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.333</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="O15" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.333</v>
+        <f t="shared" si="5"/>
+        <v/>
       </c>
       <c r="P15" s="5" t="str">
-        <f t="shared" si="7"/>
-        <v>0.667</v>
+        <f t="shared" si="6"/>
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -1100,19 +1100,19 @@
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.000</v>
       </c>
       <c r="N16" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.667</v>
       </c>
       <c r="O16" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.000</v>
       </c>
       <c r="P16" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>2.667</v>
       </c>
     </row>
@@ -1152,19 +1152,19 @@
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.333</v>
       </c>
       <c r="N17" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.333</v>
       </c>
       <c r="O17" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.500</v>
       </c>
       <c r="P17" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0.833</v>
       </c>
     </row>
@@ -1222,11 +1222,11 @@
         <v>0.881</v>
       </c>
       <c r="O18" s="6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.619</v>
       </c>
       <c r="P18" s="6" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>1.500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add SAC; Update order of columns to match scoresheet
Slight tweak to get one number right
Thanks Burch
</commit_message>
<xml_diff>
--- a/mls_f15.xlsx
+++ b/mls_f15.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Player</t>
   </si>
@@ -22,28 +22,31 @@
     <t>AB</t>
   </si>
   <si>
+    <t>R</t>
+  </si>
+  <si>
     <t>H</t>
   </si>
   <si>
-    <t>R</t>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>HR</t>
   </si>
   <si>
     <t>RBI</t>
   </si>
   <si>
-    <t>2B</t>
-  </si>
-  <si>
-    <t>3B</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
     <t>BB</t>
   </si>
   <si>
-    <t>KO</t>
+    <t>K</t>
+  </si>
+  <si>
+    <t>SAC</t>
   </si>
   <si>
     <t>AVG</t>
@@ -212,14 +215,14 @@
     <col customWidth="1" min="2" max="2" width="8.0"/>
     <col customWidth="1" min="3" max="3" width="7.14"/>
     <col customWidth="1" min="4" max="5" width="6.71"/>
-    <col customWidth="1" min="6" max="6" width="6.86"/>
-    <col customWidth="1" min="7" max="7" width="6.29"/>
-    <col customWidth="1" min="8" max="8" width="6.57"/>
-    <col customWidth="1" min="9" max="9" width="6.71"/>
+    <col customWidth="1" min="6" max="6" width="6.29"/>
+    <col customWidth="1" min="7" max="7" width="6.57"/>
+    <col customWidth="1" min="8" max="8" width="6.71"/>
+    <col customWidth="1" min="9" max="9" width="6.86"/>
     <col customWidth="1" min="10" max="10" width="7.0"/>
-    <col customWidth="1" min="11" max="11" width="7.57"/>
-    <col customWidth="1" min="12" max="12" width="4.86"/>
-    <col customWidth="1" min="13" max="16" width="8.14"/>
+    <col customWidth="1" min="11" max="12" width="7.57"/>
+    <col customWidth="1" min="13" max="13" width="4.86"/>
+    <col customWidth="1" min="14" max="17" width="8.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -256,10 +259,10 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2"/>
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
@@ -269,10 +272,13 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="str">
         <f t="shared" ref="B2:B3" si="1">4+4+3</f>
@@ -283,24 +289,24 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="str">
+        <f>3+3+2</f>
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="str">
         <f>4+2+2</f>
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="str">
-        <f>3+3+2</f>
-        <v>8</v>
-      </c>
       <c r="F2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I2" s="3">
         <v>3.0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.0</v>
       </c>
       <c r="J2" s="3">
         <v>2.0</v>
@@ -308,27 +314,30 @@
       <c r="K2" s="3">
         <v>0.0</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="5" t="str">
-        <f t="shared" ref="M2:M17" si="3">IF(C2,D2/C2,)</f>
+      <c r="L2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="5" t="str">
+        <f t="shared" ref="N2:N17" si="3">IF(C2,E2/C2,)</f>
         <v>0.889</v>
       </c>
-      <c r="N2" s="5" t="str">
-        <f t="shared" ref="N2:N17" si="4">IF(C2,((D2-G2-H2-I2)+(2*G2)+(3*H2)+(4*I2))/C2,)</f>
+      <c r="O2" s="5" t="str">
+        <f t="shared" ref="O2:O17" si="4">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
         <v>1.444</v>
       </c>
-      <c r="O2" s="5" t="str">
-        <f t="shared" ref="O2:O18" si="5">IF(B2,(D2+J2)/(C2+J2),)</f>
+      <c r="P2" s="5" t="str">
+        <f t="shared" ref="P2:P18" si="5">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
         <v>0.909</v>
       </c>
-      <c r="P2" s="5" t="str">
-        <f t="shared" ref="P2:P18" si="6">IF(N2,N2+O2,)</f>
+      <c r="Q2" s="5" t="str">
+        <f t="shared" ref="Q2:Q18" si="6">IF(O2,O2+P2,)</f>
         <v>2.354</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="str">
         <f t="shared" si="1"/>
@@ -347,48 +356,51 @@
         <v>7</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f>2+4</f>
-        <v>6</v>
-      </c>
-      <c r="G3" s="3" t="str">
         <f>2+1
 </f>
         <v>3</v>
       </c>
-      <c r="H3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="3" t="str">
+      <c r="G3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H3" s="3" t="str">
         <f>0+2</f>
         <v>2</v>
       </c>
+      <c r="I3" s="3" t="str">
+        <f>2+4</f>
+        <v>6</v>
+      </c>
       <c r="J3" s="3">
         <v>0.0</v>
       </c>
       <c r="K3" s="3">
         <v>1.0</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5" t="str">
+      <c r="L3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.636</v>
       </c>
-      <c r="N3" s="5" t="str">
+      <c r="O3" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1.455</v>
       </c>
-      <c r="O3" s="5" t="str">
+      <c r="P3" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.636</v>
       </c>
-      <c r="P3" s="5" t="str">
+      <c r="Q3" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2.091</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" ref="B4:C4" si="7">4+3+3</f>
@@ -399,54 +411,56 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="str">
-        <f>3+3+2</f>
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="str">
         <f>2+1
 </f>
         <v>3</v>
       </c>
-      <c r="F4" s="3" t="str">
+      <c r="E4" s="3">
+        <v>9.0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I4" s="3" t="str">
         <f>3+1+3</f>
         <v>7</v>
       </c>
-      <c r="G4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J4" s="3">
         <v>0.0</v>
       </c>
       <c r="K4" s="3">
         <v>0.0</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.800</v>
-      </c>
+      <c r="L4" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="4"/>
       <c r="N4" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.900</v>
       </c>
       <c r="O4" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.800</v>
+        <f t="shared" si="4"/>
+        <v>1.100</v>
       </c>
       <c r="P4" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>1.700</v>
+        <f t="shared" si="5"/>
+        <v>0.900</v>
+      </c>
+      <c r="Q4" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2.000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" ref="B5:C5" si="8">4+3
@@ -458,54 +472,56 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="str">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="3" t="str">
         <f>3+2
 </f>
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
-      </c>
       <c r="F5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="3">
         <v>5.0</v>
       </c>
-      <c r="G5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J5" s="3">
         <v>0.0</v>
       </c>
       <c r="K5" s="3">
         <v>1.0</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5" t="str">
+      <c r="L5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.714</v>
       </c>
-      <c r="N5" s="5" t="str">
+      <c r="O5" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1.571</v>
       </c>
-      <c r="O5" s="5" t="str">
+      <c r="P5" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.714</v>
       </c>
-      <c r="P5" s="5" t="str">
+      <c r="Q5" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2.286</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ref="B6:B7" si="10">4+3
@@ -527,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G6" s="3">
         <v>0.0</v>
@@ -536,7 +552,7 @@
         <v>0.0</v>
       </c>
       <c r="I6" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J6" s="3">
         <v>1.0</v>
@@ -544,27 +560,30 @@
       <c r="K6" s="3">
         <v>0.0</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5" t="str">
+      <c r="L6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.667</v>
       </c>
-      <c r="N6" s="5" t="str">
+      <c r="O6" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.667</v>
       </c>
-      <c r="O6" s="5" t="str">
+      <c r="P6" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.714</v>
       </c>
-      <c r="P6" s="5" t="str">
+      <c r="Q6" s="5" t="str">
         <f t="shared" si="6"/>
         <v>1.381</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" si="10"/>
@@ -575,55 +594,57 @@
 </f>
         <v>7</v>
       </c>
-      <c r="D7" s="3" t="str">
+      <c r="D7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E7" s="3" t="str">
         <f>3+2
 </f>
         <v>5</v>
       </c>
-      <c r="E7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F7" s="3" t="str">
-        <f>1+1
-</f>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I7" s="3" t="str">
+        <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="G7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J7" s="3">
         <v>0.0</v>
       </c>
       <c r="K7" s="3">
         <v>0.0</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5" t="str">
+      <c r="L7" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.714</v>
       </c>
-      <c r="N7" s="5" t="str">
+      <c r="O7" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1.143</v>
       </c>
-      <c r="O7" s="5" t="str">
+      <c r="P7" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.714</v>
       </c>
-      <c r="P7" s="5" t="str">
+      <c r="Q7" s="5" t="str">
         <f t="shared" si="6"/>
         <v>1.857</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>3.0</v>
@@ -632,50 +653,53 @@
         <v>3.0</v>
       </c>
       <c r="D8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E8" s="3">
         <v>2.0</v>
       </c>
-      <c r="E8" s="3">
-        <v>0.0</v>
-      </c>
       <c r="F8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="3">
         <v>2.0</v>
       </c>
-      <c r="G8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J8" s="3">
         <v>0.0</v>
       </c>
       <c r="K8" s="3">
         <v>0.0</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="5" t="str">
+      <c r="L8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.667</v>
       </c>
-      <c r="N8" s="5" t="str">
+      <c r="O8" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.667</v>
       </c>
-      <c r="O8" s="5" t="str">
+      <c r="P8" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.667</v>
       </c>
-      <c r="P8" s="5" t="str">
+      <c r="Q8" s="5" t="str">
         <f t="shared" si="6"/>
         <v>1.333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ref="B9:C9" si="11">4+4+3</f>
@@ -686,53 +710,56 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="str">
+        <f>1+2+1</f>
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="str">
         <f>2+2+2</f>
         <v>6</v>
       </c>
-      <c r="E9" s="3" t="str">
-        <f>1+2+1</f>
-        <v>4</v>
-      </c>
-      <c r="F9" s="3" t="str">
+      <c r="F9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I9" s="3" t="str">
         <f>1+1+1</f>
         <v>3</v>
       </c>
-      <c r="G9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J9" s="3">
         <v>0.0</v>
       </c>
       <c r="K9" s="3">
         <v>0.0</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="5" t="str">
+      <c r="L9" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.545</v>
       </c>
-      <c r="N9" s="5" t="str">
+      <c r="O9" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.545</v>
       </c>
-      <c r="O9" s="5" t="str">
+      <c r="P9" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.545</v>
       </c>
-      <c r="P9" s="5" t="str">
+      <c r="Q9" s="5" t="str">
         <f t="shared" si="6"/>
         <v>1.091</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ref="B10:C10" si="12">3+3+3</f>
@@ -742,54 +769,56 @@
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="D10" s="3" t="str">
+      <c r="D10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="E10" s="3" t="str">
         <f>1+1+1</f>
         <v>3</v>
       </c>
-      <c r="E10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="F10" s="3" t="str">
-        <f>1+1
-</f>
+      <c r="F10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I10" s="3" t="str">
+        <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="G10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J10" s="3">
         <v>0.0</v>
       </c>
       <c r="K10" s="3">
         <v>0.0</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="5" t="str">
+      <c r="L10" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="N10" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.333</v>
       </c>
-      <c r="N10" s="5" t="str">
+      <c r="O10" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.444</v>
       </c>
-      <c r="O10" s="5" t="str">
+      <c r="P10" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.333</v>
       </c>
-      <c r="P10" s="5" t="str">
+      <c r="Q10" s="5" t="str">
         <f t="shared" si="6"/>
         <v>0.778</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" ref="B11:C11" si="13">3+3+3</f>
@@ -800,169 +829,177 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="str">
+        <f>2+1+1</f>
+        <v>4</v>
+      </c>
+      <c r="E11" s="3" t="str">
         <f>2+2
 </f>
         <v>4</v>
       </c>
-      <c r="E11" s="3" t="str">
-        <f t="shared" ref="E11:F11" si="14">2+1+1</f>
+      <c r="F11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="3" t="str">
+        <f>2+1+1</f>
         <v>4</v>
       </c>
-      <c r="F11" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v>4</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J11" s="3">
         <v>0.0</v>
       </c>
       <c r="K11" s="3">
         <v>0.0</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="5" t="str">
+      <c r="L11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="4"/>
+      <c r="N11" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.444</v>
       </c>
-      <c r="N11" s="5" t="str">
+      <c r="O11" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.778</v>
       </c>
-      <c r="O11" s="5" t="str">
+      <c r="P11" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.444</v>
       </c>
-      <c r="P11" s="5" t="str">
+      <c r="Q11" s="5" t="str">
         <f t="shared" si="6"/>
         <v>1.222</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f t="shared" ref="B12:C12" si="15">3+3+3</f>
+        <f t="shared" ref="B12:C12" si="14">3+3+3</f>
         <v>9</v>
       </c>
       <c r="C12" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+      <c r="E12" s="3" t="str">
+        <f>1+2+1</f>
+        <v>4</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="4"/>
+      <c r="N12" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.444</v>
+      </c>
+      <c r="O12" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>0.444</v>
+      </c>
+      <c r="P12" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>0.444</v>
+      </c>
+      <c r="Q12" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>0.889</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f t="shared" ref="B13:C13" si="15">3+3+3</f>
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="str">
         <f t="shared" si="15"/>
         <v>9</v>
       </c>
-      <c r="D12" s="3" t="str">
-        <f>1+2+1</f>
-        <v>4</v>
-      </c>
-      <c r="E12" s="3" t="str">
-        <f>1+1
-</f>
-        <v>2</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="J12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.444</v>
-      </c>
-      <c r="N12" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.444</v>
-      </c>
-      <c r="O12" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.444</v>
-      </c>
-      <c r="P12" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.889</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3" t="str">
-        <f t="shared" ref="B13:C13" si="16">3+3+3</f>
-        <v>9</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v>9</v>
-      </c>
       <c r="D13" s="3" t="str">
-        <f>2+2+1</f>
-        <v>5</v>
-      </c>
-      <c r="E13" s="3" t="str">
         <f>2+1
 </f>
         <v>3</v>
       </c>
-      <c r="F13" s="3" t="str">
+      <c r="E13" s="3" t="str">
+        <f>2+2+1</f>
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I13" s="3" t="str">
         <f>0+2</f>
         <v>2</v>
       </c>
-      <c r="G13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J13" s="3">
         <v>0.0</v>
       </c>
       <c r="K13" s="3">
         <v>0.0</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="5" t="str">
+      <c r="L13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.556</v>
       </c>
-      <c r="N13" s="5" t="str">
+      <c r="O13" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.556</v>
       </c>
-      <c r="O13" s="5" t="str">
+      <c r="P13" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.556</v>
       </c>
-      <c r="P13" s="5" t="str">
+      <c r="Q13" s="5" t="str">
         <f t="shared" si="6"/>
         <v>1.111</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3">
         <v>3.0</v>
@@ -971,10 +1008,10 @@
         <v>3.0</v>
       </c>
       <c r="D14" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E14" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="F14" s="3">
         <v>0.0</v>
@@ -994,27 +1031,30 @@
       <c r="K14" s="3">
         <v>0.0</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="5" t="str">
+      <c r="L14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="4"/>
+      <c r="N14" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.333</v>
       </c>
-      <c r="N14" s="5" t="str">
+      <c r="O14" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.333</v>
       </c>
-      <c r="O14" s="5" t="str">
+      <c r="P14" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.333</v>
       </c>
-      <c r="P14" s="5" t="str">
+      <c r="Q14" s="5" t="str">
         <f t="shared" si="6"/>
         <v>0.667</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>0.0</v>
@@ -1046,27 +1086,30 @@
       <c r="K15" s="3">
         <v>0.0</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="5" t="str">
+      <c r="L15" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="5" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="N15" s="5" t="str">
+      <c r="O15" s="5" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O15" s="5" t="str">
+      <c r="P15" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="P15" s="5" t="str">
+      <c r="Q15" s="5" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3">
         <v>3.0</v>
@@ -1075,50 +1118,53 @@
         <v>3.0</v>
       </c>
       <c r="D16" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E16" s="3">
         <v>3.0</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>2.0</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I16" s="3">
         <v>3.0</v>
       </c>
-      <c r="G16" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.0</v>
-      </c>
       <c r="J16" s="3">
         <v>0.0</v>
       </c>
       <c r="K16" s="3">
         <v>0.0</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="5" t="str">
+      <c r="L16" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="5" t="str">
         <f t="shared" si="3"/>
         <v>1.000</v>
       </c>
-      <c r="N16" s="5" t="str">
+      <c r="O16" s="5" t="str">
         <f t="shared" si="4"/>
         <v>1.667</v>
       </c>
-      <c r="O16" s="5" t="str">
+      <c r="P16" s="5" t="str">
         <f t="shared" si="5"/>
         <v>1.000</v>
       </c>
-      <c r="P16" s="5" t="str">
+      <c r="Q16" s="5" t="str">
         <f t="shared" si="6"/>
         <v>2.667</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3">
         <v>4.0</v>
@@ -1133,7 +1179,7 @@
         <v>1.0</v>
       </c>
       <c r="F17" s="3">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="G17" s="3">
         <v>0.0</v>
@@ -1142,7 +1188,7 @@
         <v>0.0</v>
       </c>
       <c r="I17" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J17" s="3">
         <v>1.0</v>
@@ -1150,88 +1196,98 @@
       <c r="K17" s="3">
         <v>0.0</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="5" t="str">
+      <c r="L17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="5" t="str">
         <f t="shared" si="3"/>
         <v>0.333</v>
       </c>
-      <c r="N17" s="5" t="str">
+      <c r="O17" s="5" t="str">
         <f t="shared" si="4"/>
         <v>0.333</v>
       </c>
-      <c r="O17" s="5" t="str">
+      <c r="P17" s="5" t="str">
         <f t="shared" si="5"/>
         <v>0.500</v>
       </c>
-      <c r="P17" s="5" t="str">
+      <c r="Q17" s="5" t="str">
         <f t="shared" si="6"/>
         <v>0.833</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:K18" si="17">sum(B2:B17)</f>
+        <f t="shared" ref="B18:L18" si="16">sum(B2:B17)</f>
         <v>113</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>109</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>66</v>
+        <f t="shared" si="16"/>
+        <v>42</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
+        <v>67</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="16"/>
         <v>42</v>
       </c>
-      <c r="F18" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>42</v>
-      </c>
-      <c r="G18" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>11</v>
-      </c>
-      <c r="H18" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>5</v>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f t="shared" si="17"/>
-        <v>3</v>
-      </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="6" t="str">
-        <f>D18/C18</f>
-        <v>0.606</v>
-      </c>
+      <c r="L18" s="1" t="str">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="3"/>
       <c r="N18" s="6" t="str">
-        <f>((D18-G18-H18-I18)+(2*G18)+(3*H18)+(4*I18))/C18</f>
-        <v>0.881</v>
+        <f>E18/C18</f>
+        <v>0.615</v>
       </c>
       <c r="O18" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>0.619</v>
+        <f>((E18-F18-G18-H18)+(2*F18)+(3*G18)+(4*H18))/C18</f>
+        <v>0.899</v>
       </c>
       <c r="P18" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>1.500</v>
+        <f t="shared" si="5"/>
+        <v>0.628</v>
+      </c>
+      <c r="Q18" s="6" t="str">
+        <f t="shared" si="6"/>
+        <v>1.527</v>
       </c>
     </row>
     <row r="22">
-      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23">
+      <c r="G23" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update stats after 10/7/15 game
</commit_message>
<xml_diff>
--- a/mls_f15.xlsx
+++ b/mls_f15.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Copy of Fall 2015" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -281,20 +281,20 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f t="shared" ref="B2:B3" si="1">4+4+3</f>
+        <f t="shared" ref="B2:B3" si="1">4+4+3+5</f>
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f>4+2+3+5</f>
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>3+3+2+3</f>
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="str">
-        <f>4+2+3</f>
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="str">
-        <f>3+3+2</f>
-        <v>8</v>
-      </c>
       <c r="E2" s="3" t="str">
-        <f>4+2+2</f>
-        <v>8</v>
+        <f>4+2+2+4</f>
+        <v>12</v>
       </c>
       <c r="F2" s="3">
         <v>2.0</v>
@@ -305,8 +305,10 @@
       <c r="H2" s="3">
         <v>1.0</v>
       </c>
-      <c r="I2" s="3">
-        <v>3.0</v>
+      <c r="I2" s="3" t="str">
+        <f>3+4
+</f>
+        <v>7</v>
       </c>
       <c r="J2" s="3">
         <v>2.0</v>
@@ -319,20 +321,20 @@
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="5" t="str">
-        <f t="shared" ref="N2:N17" si="3">IF(C2,E2/C2,)</f>
-        <v>0.889</v>
+        <f t="shared" ref="N2:N17" si="2">IF(C2,E2/C2,)</f>
+        <v>0.857</v>
       </c>
       <c r="O2" s="5" t="str">
-        <f t="shared" ref="O2:O17" si="4">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
-        <v>1.444</v>
+        <f t="shared" ref="O2:O17" si="3">IF(C2,((E2-F2-G2-H2)+(2*F2)+(3*G2)+(4*H2))/C2,)</f>
+        <v>1.214</v>
       </c>
       <c r="P2" s="5" t="str">
-        <f t="shared" ref="P2:P18" si="5">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
-        <v>0.909</v>
+        <f t="shared" ref="P2:P18" si="4">IF(B2,(E2+J2)/(C2+J2+L2),)</f>
+        <v>0.875</v>
       </c>
       <c r="Q2" s="5" t="str">
-        <f t="shared" ref="Q2:Q18" si="6">IF(O2,O2+P2,)</f>
-        <v>2.354</v>
+        <f t="shared" ref="Q2:Q18" si="5">IF(O2,O2+P2,)</f>
+        <v>2.089</v>
       </c>
     </row>
     <row r="3">
@@ -341,19 +343,19 @@
       </c>
       <c r="B3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="str">
-        <f>4+4+3</f>
-        <v>11</v>
+        <f>4+4+3+3</f>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="str">
-        <f t="shared" ref="D3:E3" si="2">3+3+1</f>
-        <v>7</v>
+        <f>3+3+1+1</f>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f>3+3+1+2</f>
+        <v>9</v>
       </c>
       <c r="F3" s="3" t="str">
         <f>2+1
@@ -368,8 +370,8 @@
         <v>2</v>
       </c>
       <c r="I3" s="3" t="str">
-        <f>2+4</f>
-        <v>6</v>
+        <f>2+4+2</f>
+        <v>8</v>
       </c>
       <c r="J3" s="3">
         <v>0.0</v>
@@ -378,24 +380,24 @@
         <v>1.0</v>
       </c>
       <c r="L3" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.636</v>
+        <f t="shared" si="2"/>
+        <v>0.643</v>
       </c>
       <c r="O3" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.455</v>
+        <f t="shared" si="3"/>
+        <v>1.286</v>
       </c>
       <c r="P3" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.636</v>
+        <f t="shared" si="4"/>
+        <v>0.600</v>
       </c>
       <c r="Q3" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>2.091</v>
+        <f t="shared" si="5"/>
+        <v>1.886</v>
       </c>
     </row>
     <row r="4">
@@ -403,20 +405,22 @@
         <v>18</v>
       </c>
       <c r="B4" s="3" t="str">
-        <f t="shared" ref="B4:C4" si="7">4+3+3</f>
-        <v>10</v>
+        <f t="shared" ref="B4:C4" si="6">4+3+3+4</f>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="str">
         <f>2+1
 </f>
         <v>3</v>
       </c>
-      <c r="E4" s="3">
-        <v>9.0</v>
+      <c r="E4" s="3" t="str">
+        <f>9+2
+</f>
+        <v>11</v>
       </c>
       <c r="F4" s="3">
         <v>2.0</v>
@@ -428,8 +432,8 @@
         <v>0.0</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f>3+1+3</f>
-        <v>7</v>
+        <f>3+1+3+1</f>
+        <v>8</v>
       </c>
       <c r="J4" s="3">
         <v>0.0</v>
@@ -442,20 +446,20 @@
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.900</v>
+        <f t="shared" si="2"/>
+        <v>0.786</v>
       </c>
       <c r="O4" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.100</v>
+        <f t="shared" si="3"/>
+        <v>0.929</v>
       </c>
       <c r="P4" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.900</v>
+        <f t="shared" si="4"/>
+        <v>0.786</v>
       </c>
       <c r="Q4" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>2.000</v>
+        <f t="shared" si="5"/>
+        <v>1.714</v>
       </c>
     </row>
     <row r="5">
@@ -463,25 +467,26 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="str">
-        <f t="shared" ref="B5:C5" si="8">4+3
-</f>
-        <v>7</v>
+        <f>4+3+4</f>
+        <v>11</v>
       </c>
       <c r="C5" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>7</v>
+        <f>4+3+3
+</f>
+        <v>10</v>
       </c>
       <c r="D5" s="3" t="str">
-        <f>1+1</f>
-        <v>2</v>
+        <f>1+1+3</f>
+        <v>5</v>
       </c>
       <c r="E5" s="3" t="str">
-        <f>3+2
-</f>
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.0</v>
+        <f>3+2+3
+</f>
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="G5" s="3">
         <v>3.0</v>
@@ -489,8 +494,10 @@
       <c r="H5" s="3">
         <v>0.0</v>
       </c>
-      <c r="I5" s="3">
-        <v>5.0</v>
+      <c r="I5" s="3" t="str">
+        <f>5+4
+</f>
+        <v>9</v>
       </c>
       <c r="J5" s="3">
         <v>0.0</v>
@@ -499,24 +506,24 @@
         <v>1.0</v>
       </c>
       <c r="L5" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.714</v>
+        <f t="shared" si="2"/>
+        <v>0.800</v>
       </c>
       <c r="O5" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.571</v>
+        <f t="shared" si="3"/>
+        <v>1.500</v>
       </c>
       <c r="P5" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.714</v>
+        <f t="shared" si="4"/>
+        <v>0.727</v>
       </c>
       <c r="Q5" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>2.286</v>
+        <f t="shared" si="5"/>
+        <v>2.227</v>
       </c>
     </row>
     <row r="6">
@@ -524,7 +531,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="3" t="str">
-        <f t="shared" ref="B6:B7" si="10">4+3
+        <f>4+3
 </f>
         <v>7</v>
       </c>
@@ -534,12 +541,12 @@
         <v>6</v>
       </c>
       <c r="D6" s="3" t="str">
-        <f t="shared" ref="D6:E6" si="9">2+2
+        <f t="shared" ref="D6:E6" si="7">2+2
 </f>
         <v>4</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="F6" s="3">
@@ -565,19 +572,19 @@
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.667</v>
       </c>
       <c r="O6" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.667</v>
       </c>
       <c r="P6" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.714</v>
       </c>
       <c r="Q6" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.381</v>
       </c>
     </row>
@@ -586,24 +593,27 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>7</v>
+        <f t="shared" ref="B7:C7" si="8">4+3+4</f>
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="str">
-        <f>4+3
-</f>
-        <v>7</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1.0</v>
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>1+3
+</f>
+        <v>4</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>3+2
-</f>
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1.0</v>
+        <f>3+2+3
+</f>
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f>1+2
+</f>
+        <v>3</v>
       </c>
       <c r="G7" s="3">
         <v>1.0</v>
@@ -612,8 +622,8 @@
         <v>0.0</v>
       </c>
       <c r="I7" s="3" t="str">
-        <f>1+1</f>
-        <v>2</v>
+        <f>1+1+2</f>
+        <v>4</v>
       </c>
       <c r="J7" s="3">
         <v>0.0</v>
@@ -626,37 +636,42 @@
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.714</v>
+        <f t="shared" si="2"/>
+        <v>0.727</v>
       </c>
       <c r="O7" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>1.143</v>
+        <f t="shared" si="3"/>
+        <v>1.182</v>
       </c>
       <c r="P7" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.714</v>
+        <f t="shared" si="4"/>
+        <v>0.727</v>
       </c>
       <c r="Q7" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>1.857</v>
+        <f t="shared" si="5"/>
+        <v>1.909</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="3" t="str">
+        <f t="shared" ref="B8:C8" si="9">3+4
+</f>
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
         <v>3.0</v>
       </c>
-      <c r="C8" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2.0</v>
+      <c r="E8" s="3" t="str">
+        <f>2+3
+</f>
+        <v>5</v>
       </c>
       <c r="F8" s="3">
         <v>0.0</v>
@@ -667,8 +682,10 @@
       <c r="H8" s="3">
         <v>0.0</v>
       </c>
-      <c r="I8" s="3">
-        <v>2.0</v>
+      <c r="I8" s="3" t="str">
+        <f>2+2
+</f>
+        <v>4</v>
       </c>
       <c r="J8" s="3">
         <v>0.0</v>
@@ -681,20 +698,20 @@
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.667</v>
+        <f t="shared" si="2"/>
+        <v>0.714</v>
       </c>
       <c r="O8" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.667</v>
+        <f t="shared" si="3"/>
+        <v>0.714</v>
       </c>
       <c r="P8" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.667</v>
+        <f t="shared" si="4"/>
+        <v>0.714</v>
       </c>
       <c r="Q8" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>1.333</v>
+        <f t="shared" si="5"/>
+        <v>1.429</v>
       </c>
     </row>
     <row r="9">
@@ -702,11 +719,11 @@
         <v>23</v>
       </c>
       <c r="B9" s="3" t="str">
-        <f t="shared" ref="B9:C9" si="11">4+4+3</f>
+        <f t="shared" ref="B9:C9" si="10">4+4+3</f>
         <v>11</v>
       </c>
       <c r="C9" s="3" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="D9" s="3" t="str">
@@ -741,19 +758,19 @@
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.545</v>
       </c>
       <c r="O9" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.545</v>
       </c>
       <c r="P9" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.545</v>
       </c>
       <c r="Q9" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>1.091</v>
       </c>
     </row>
@@ -762,19 +779,21 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="str">
-        <f t="shared" ref="B10:C10" si="12">3+3+3</f>
-        <v>9</v>
+        <f t="shared" ref="B10:C10" si="11">3+3+3+4</f>
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="str">
-        <f t="shared" si="12"/>
-        <v>9</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.0</v>
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f>1+2
+</f>
+        <v>3</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f>1+1+1</f>
-        <v>3</v>
+        <f>1+1+1+3</f>
+        <v>6</v>
       </c>
       <c r="F10" s="3">
         <v>1.0</v>
@@ -786,8 +805,8 @@
         <v>0.0</v>
       </c>
       <c r="I10" s="3" t="str">
-        <f>1+1</f>
-        <v>2</v>
+        <f>1+1+2</f>
+        <v>4</v>
       </c>
       <c r="J10" s="3">
         <v>0.0</v>
@@ -800,20 +819,20 @@
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.333</v>
+        <f t="shared" si="2"/>
+        <v>0.462</v>
       </c>
       <c r="O10" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.444</v>
+        <f t="shared" si="3"/>
+        <v>0.538</v>
       </c>
       <c r="P10" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.333</v>
+        <f t="shared" si="4"/>
+        <v>0.462</v>
       </c>
       <c r="Q10" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.778</v>
+        <f t="shared" si="5"/>
+        <v>1.000</v>
       </c>
     </row>
     <row r="11">
@@ -821,24 +840,26 @@
         <v>25</v>
       </c>
       <c r="B11" s="3" t="str">
-        <f t="shared" ref="B11:C11" si="13">3+3+3</f>
-        <v>9</v>
+        <f t="shared" ref="B11:C11" si="12">3+3+3+4</f>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>9</v>
+        <f t="shared" si="12"/>
+        <v>13</v>
       </c>
       <c r="D11" s="3" t="str">
-        <f>2+1+1</f>
-        <v>4</v>
+        <f>2+1+1+4</f>
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f>2+2
-</f>
-        <v>4</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1.0</v>
+        <f>2+2+4
+</f>
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f>1+1
+</f>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
         <v>1.0</v>
@@ -847,8 +868,8 @@
         <v>0.0</v>
       </c>
       <c r="I11" s="3" t="str">
-        <f>2+1+1</f>
-        <v>4</v>
+        <f>2+1+1+3</f>
+        <v>7</v>
       </c>
       <c r="J11" s="3">
         <v>0.0</v>
@@ -861,20 +882,20 @@
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.444</v>
+        <f t="shared" si="2"/>
+        <v>0.615</v>
       </c>
       <c r="O11" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.778</v>
+        <f t="shared" si="3"/>
+        <v>0.923</v>
       </c>
       <c r="P11" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.444</v>
+        <f t="shared" si="4"/>
+        <v>0.615</v>
       </c>
       <c r="Q11" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>1.222</v>
+        <f t="shared" si="5"/>
+        <v>1.538</v>
       </c>
     </row>
     <row r="12">
@@ -882,32 +903,34 @@
         <v>26</v>
       </c>
       <c r="B12" s="3" t="str">
-        <f t="shared" ref="B12:C12" si="14">3+3+3</f>
-        <v>9</v>
+        <f t="shared" ref="B12:C12" si="13">3+3+3+4</f>
+        <v>13</v>
       </c>
       <c r="C12" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v>9</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="D12" s="3" t="str">
-        <f>1+1</f>
-        <v>2</v>
+        <f>1+1+3</f>
+        <v>5</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>1+2+1</f>
+        <f>1+2+1+3</f>
+        <v>7</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I12" s="3" t="str">
+        <f>1+3
+</f>
         <v>4</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I12" s="3">
-        <v>1.0</v>
       </c>
       <c r="J12" s="3">
         <v>0.0</v>
@@ -920,20 +943,20 @@
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.444</v>
+        <f t="shared" si="2"/>
+        <v>0.538</v>
       </c>
       <c r="O12" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.444</v>
+        <f t="shared" si="3"/>
+        <v>0.538</v>
       </c>
       <c r="P12" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.444</v>
+        <f t="shared" si="4"/>
+        <v>0.538</v>
       </c>
       <c r="Q12" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.889</v>
+        <f t="shared" si="5"/>
+        <v>1.077</v>
       </c>
     </row>
     <row r="13">
@@ -941,34 +964,35 @@
         <v>27</v>
       </c>
       <c r="B13" s="3" t="str">
-        <f t="shared" ref="B13:C13" si="15">3+3+3</f>
-        <v>9</v>
+        <f t="shared" ref="B13:C13" si="14">3+3+3+4</f>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v>9</v>
+        <f t="shared" si="14"/>
+        <v>13</v>
       </c>
       <c r="D13" s="3" t="str">
-        <f>2+1
-</f>
-        <v>3</v>
+        <f>2+1+3
+</f>
+        <v>6</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f>2+2+1</f>
+        <f>2+2+1+3</f>
+        <v>8</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I13" s="3" t="str">
+        <f>2+3
+</f>
         <v>5</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="I13" s="3" t="str">
-        <f>0+2</f>
-        <v>2</v>
       </c>
       <c r="J13" s="3">
         <v>0.0</v>
@@ -981,37 +1005,42 @@
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.556</v>
+        <f t="shared" si="2"/>
+        <v>0.615</v>
       </c>
       <c r="O13" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.556</v>
+        <f t="shared" si="3"/>
+        <v>0.615</v>
       </c>
       <c r="P13" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.556</v>
+        <f t="shared" si="4"/>
+        <v>0.615</v>
       </c>
       <c r="Q13" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>1.111</v>
+        <f t="shared" si="5"/>
+        <v>1.231</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="3" t="str">
+        <f t="shared" ref="B14:C14" si="15">3+4
+</f>
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="D14" s="3">
         <v>3.0</v>
       </c>
-      <c r="C14" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1.0</v>
+      <c r="E14" s="3" t="str">
+        <f>1+3
+</f>
+        <v>4</v>
       </c>
       <c r="F14" s="3">
         <v>0.0</v>
@@ -1023,7 +1052,7 @@
         <v>0.0</v>
       </c>
       <c r="I14" s="3">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J14" s="3">
         <v>0.0</v>
@@ -1036,40 +1065,45 @@
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v>0.333</v>
+        <f t="shared" si="2"/>
+        <v>0.571</v>
       </c>
       <c r="O14" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v>0.333</v>
+        <f t="shared" si="3"/>
+        <v>0.571</v>
       </c>
       <c r="P14" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v>0.333</v>
+        <f t="shared" si="4"/>
+        <v>0.571</v>
       </c>
       <c r="Q14" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v>0.667</v>
+        <f t="shared" si="5"/>
+        <v>1.143</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.0</v>
+      <c r="B15" s="3" t="str">
+        <f t="shared" ref="B15:C15" si="16">4</f>
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="E15" s="3" t="str">
+        <f>3</f>
+        <v>3</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f>1</f>
+        <v>1</v>
       </c>
       <c r="G15" s="3">
         <v>0.0</v>
@@ -1077,8 +1111,9 @@
       <c r="H15" s="3">
         <v>0.0</v>
       </c>
-      <c r="I15" s="3">
-        <v>0.0</v>
+      <c r="I15" s="3" t="str">
+        <f>3</f>
+        <v>3</v>
       </c>
       <c r="J15" s="3">
         <v>0.0</v>
@@ -1091,20 +1126,20 @@
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="5" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>0.750</v>
       </c>
       <c r="O15" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>1.000</v>
       </c>
       <c r="P15" s="5" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>0.750</v>
       </c>
       <c r="Q15" s="5" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+        <f t="shared" si="5"/>
+        <v>1.750</v>
       </c>
     </row>
     <row r="16">
@@ -1146,19 +1181,19 @@
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.000</v>
       </c>
       <c r="O16" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.667</v>
       </c>
       <c r="P16" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.000</v>
       </c>
       <c r="Q16" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2.667</v>
       </c>
     </row>
@@ -1201,19 +1236,19 @@
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.333</v>
       </c>
       <c r="O17" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.333</v>
       </c>
       <c r="P17" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.500</v>
       </c>
       <c r="Q17" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.833</v>
       </c>
     </row>
@@ -1222,65 +1257,65 @@
         <v>32</v>
       </c>
       <c r="B18" s="1" t="str">
-        <f t="shared" ref="B18:L18" si="16">sum(B2:B17)</f>
-        <v>113</v>
+        <f t="shared" ref="B18:L18" si="17">sum(B2:B17)</f>
+        <v>163</v>
       </c>
       <c r="C18" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>109</v>
+        <f t="shared" si="17"/>
+        <v>156</v>
       </c>
       <c r="D18" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>42</v>
+        <f t="shared" si="17"/>
+        <v>72</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>67</v>
+        <f t="shared" si="17"/>
+        <v>103</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>12</v>
+        <f t="shared" si="17"/>
+        <v>17</v>
       </c>
       <c r="G18" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="H18" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>42</v>
+        <f t="shared" si="17"/>
+        <v>72</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="L18" s="1" t="str">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>2</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="6" t="str">
         <f>E18/C18</f>
-        <v>0.615</v>
+        <v>0.660</v>
       </c>
       <c r="O18" s="6" t="str">
         <f>((E18-F18-G18-H18)+(2*F18)+(3*G18)+(4*H18))/C18</f>
-        <v>0.899</v>
+        <v>0.891</v>
       </c>
       <c r="P18" s="6" t="str">
-        <f t="shared" si="5"/>
-        <v>0.628</v>
+        <f t="shared" si="4"/>
+        <v>0.660</v>
       </c>
       <c r="Q18" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>1.527</v>
+        <f t="shared" si="5"/>
+        <v>1.552</v>
       </c>
     </row>
     <row r="22">

</xml_diff>